<commit_message>
imported data into ipynb
</commit_message>
<xml_diff>
--- a/State codes.xlsx
+++ b/State codes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Other\Documents\Projects_Repos\GitHUb_Homeworks\Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/35f71590851144db/Homework/Project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{076C5729-5E15-4EF7-AAA4-CFEFF037EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{7AE18B1C-CA2F-48B5-8085-223F0A16C72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D473853-31B2-4581-A911-32F68CBA89F8}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{76448862-E8AC-48C8-BB90-A19660856F65}"/>
+    <workbookView xWindow="13785" yWindow="-10635" windowWidth="7740" windowHeight="9420" xr2:uid="{76448862-E8AC-48C8-BB90-A19660856F65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>STATE</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>WB</t>
-  </si>
-  <si>
-    <t>UNION TERRITORY</t>
   </si>
   <si>
     <t>ANDAMAN &amp; NICOBAR</t>
@@ -317,10 +314,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,18 +632,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DD830B-7C25-44A4-B0DE-B0AED0BCFBAB}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="41.65">
+    <row r="1" spans="1:2" ht="42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,304 +651,296 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" ht="28">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="4" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="4" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="4" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="4" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="4" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="4" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="4" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="4" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="4" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="4" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="4" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="4" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="4" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="4" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="4" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="4" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="4" t="s">
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="4" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="4" t="s">
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="4" t="s">
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="4" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="55.5">
-      <c r="A29" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4" t="s">
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="41.65">
-      <c r="A32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B28:B29"/>
-  </mergeCells>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B37">
+    <sortCondition ref="A4:A37"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>